<commit_message>
UPDATED LP HW for 18 and 19
</commit_message>
<xml_diff>
--- a/01-Lesson-Plans/18-Blockchain/3/TimeTracker.xlsx
+++ b/01-Lesson-Plans/18-Blockchain/3/TimeTracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/torturedgenius/trilogy/FinTech/FinTech-Lesson-Plans/01-Lesson-Plans/18-Blockchain/3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lorie\Bootcamp\FinTech\FinTech-Lesson-Plans\01-Lesson-Plans\18-Blockchain\3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4729B777-B153-FF44-A54D-4A1FA8A0908A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E676B2F0-9C2E-4442-8B7F-2402E2F6E5B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="19400" windowHeight="17840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Weeknight" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -29,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="31">
-  <si>
-    <t>Lesson Plan 18.3 - Time Tracker</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
   <si>
     <t>Time</t>
   </si>
@@ -52,61 +51,7 @@
     <t>6:30 PM</t>
   </si>
   <si>
-    <t>Instructor Do: Welcome Class</t>
-  </si>
-  <si>
-    <t>0:10</t>
-  </si>
-  <si>
-    <t>Instructor Do: Consensus Algorithms</t>
-  </si>
-  <si>
-    <t>Students Do: Turn and Teach Consensus Algorithms</t>
-  </si>
-  <si>
-    <t>0:15</t>
-  </si>
-  <si>
-    <t>Instructor Do: Consensus Algorithm Review</t>
-  </si>
-  <si>
-    <t>0:05</t>
-  </si>
-  <si>
-    <t>Instructor Do: Creating a Genesis Block Demo</t>
-  </si>
-  <si>
-    <t>Students Do: Creating a Genesis Block</t>
-  </si>
-  <si>
-    <t>Instructor Do: Creating a Genesis Block Review</t>
-  </si>
-  <si>
-    <t>Instructor Do: Creating two nodes with accounts</t>
-  </si>
-  <si>
-    <t>Students Do: Creating two nodes with accounts</t>
-  </si>
-  <si>
-    <t>Instructor Do: Review Node configuration</t>
-  </si>
-  <si>
     <t>BREAK</t>
-  </si>
-  <si>
-    <t>Instructor Do: Starting the Blockchain</t>
-  </si>
-  <si>
-    <t>Students Do: Bringing the blockchain to life</t>
-  </si>
-  <si>
-    <t>Instructor Do: Ensuring Block Production</t>
-  </si>
-  <si>
-    <t>Instructor Do: Transacting on the chain</t>
-  </si>
-  <si>
-    <t>Students Do: Transacting on their chains</t>
   </si>
   <si>
     <t>END</t>
@@ -115,20 +60,47 @@
     <t>10:00 AM</t>
   </si>
   <si>
-    <t>0:40</t>
-  </si>
-  <si>
     <t>Instructor Do: Structured Review</t>
   </si>
   <si>
-    <t>0:35</t>
+    <t>Lesson Plan 18.3 - Time Tracker</t>
+  </si>
+  <si>
+    <t>Instructor Do: Decentralized Systems</t>
+  </si>
+  <si>
+    <t>Instructor Do: Components of a Blockchain System</t>
+  </si>
+  <si>
+    <t>Instructor Do: Hash Guesser</t>
+  </si>
+  <si>
+    <t>Everyone Do: Add Hashing to a Block</t>
+  </si>
+  <si>
+    <t>Everyone Do: Integrate Proof of Work into PyChain</t>
+  </si>
+  <si>
+    <t>Student Do: Dynamic Difficulty</t>
+  </si>
+  <si>
+    <t>Instructor Do: Review Dynamic Difficulty</t>
+  </si>
+  <si>
+    <t>Instructor Do: Proof of Work Validation</t>
+  </si>
+  <si>
+    <t>Student Do: Validating the Blockchain</t>
+  </si>
+  <si>
+    <t>Instructor Do: Review Validating the Blockchain</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,6 +115,38 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -162,26 +166,252 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="18" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Excel Built-in Normal" xfId="1" xr:uid="{C5CD0348-3A6D-44F0-AEBB-2E737FFFEAA8}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="99">
+  <dxfs count="129">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDDDDDD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDDDDDD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDDDDDD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDDDDDD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDDDDDD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDDDDDD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDDDDDD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDDDDDD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDDDDDD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDDDDDD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1209,13 +1439,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="10.6640625" customWidth="1"/>
     <col min="3" max="3" width="50.6640625" customWidth="1"/>
@@ -1223,473 +1453,357 @@
     <col min="5" max="5" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="5">
+        <v>6.9444444444444449E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
-        <f t="shared" ref="A4:A19" si="0">IF(LOWER($E3)="skip",A3,A3+D3)</f>
+        <f t="shared" ref="A4:A14" si="0">IF(LOWER($E3)="skip",A3,A3+D3)</f>
         <v>0.77777777777777779</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="5">
+        <v>1.3888888888888888E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <f t="shared" si="0"/>
-        <v>0.78472222222222221</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="B5" s="1">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="5">
+        <v>1.0416666666666666E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <f t="shared" si="0"/>
-        <v>0.79513888888888884</v>
+        <v>0.80208333333333326</v>
       </c>
       <c r="B6" s="1">
         <v>4</v>
       </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="5">
+        <v>1.3888888888888888E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
-        <v>0.79861111111111105</v>
+        <v>0.8159722222222221</v>
       </c>
       <c r="B7" s="1">
         <v>5</v>
       </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="6">
+        <v>1.3888888888888888E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
-        <v>0.80555555555555547</v>
+        <v>0.82986111111111094</v>
       </c>
       <c r="B8" s="1">
         <v>6</v>
       </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="7">
+        <v>1.3888888888888888E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
-        <v>0.81249999999999989</v>
+        <v>0.84374999999999978</v>
       </c>
       <c r="B9" s="1">
         <v>7</v>
       </c>
-      <c r="C9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="5">
+        <v>6.9444444444444449E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
-        <v>0.8159722222222221</v>
+        <v>0.8506944444444442</v>
       </c>
       <c r="B10" s="1">
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="D10" s="8">
+        <v>1.0416666666666666E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
-        <v>0.82291666666666652</v>
+        <v>0.86111111111111083</v>
       </c>
       <c r="B11" s="1">
         <v>9</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D11" s="5">
+        <v>1.3888888888888888E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
-        <v>0.83333333333333315</v>
+        <v>0.87499999999999967</v>
       </c>
       <c r="B12" s="1">
         <v>10</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D12" s="7">
+        <v>1.3888888888888888E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
-        <v>0.84374999999999978</v>
+        <v>0.88888888888888851</v>
       </c>
       <c r="B13" s="1">
         <v>11</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D13" s="5">
+        <v>6.9444444444444441E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
-        <v>0.85416666666666641</v>
+        <v>0.89583333333333293</v>
       </c>
       <c r="B14" s="1">
-        <v>12</v>
-      </c>
-      <c r="C14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
-        <f t="shared" si="0"/>
-        <v>0.86111111111111083</v>
-      </c>
-      <c r="B15" s="1">
-        <v>13</v>
-      </c>
-      <c r="C15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
-        <f t="shared" si="0"/>
-        <v>0.87152777777777746</v>
-      </c>
-      <c r="B16" s="1">
-        <v>14</v>
-      </c>
-      <c r="C16" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
-        <f t="shared" si="0"/>
-        <v>0.88194444444444409</v>
-      </c>
-      <c r="B17" s="1">
         <v>15</v>
       </c>
-      <c r="C17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
-        <f t="shared" si="0"/>
-        <v>0.88888888888888851</v>
-      </c>
-      <c r="B18" s="1">
-        <v>16</v>
-      </c>
-      <c r="C18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
-        <f t="shared" si="0"/>
-        <v>0.89583333333333293</v>
-      </c>
-      <c r="C19" t="s">
-        <v>26</v>
-      </c>
+      <c r="C14" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="2"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A10:E10">
-    <cfRule type="expression" dxfId="98" priority="22">
+  <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="E11:E15 A10:E10 D13 A11:B14 A15:A17">
+    <cfRule type="expression" dxfId="128" priority="22">
       <formula>LOWER($E10)="critical"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="97" priority="23">
+    <cfRule type="expression" dxfId="127" priority="23">
       <formula>LOWER($E10)="high"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="96" priority="24">
+    <cfRule type="expression" dxfId="126" priority="24">
       <formula>LOWER($E10)="skip"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A11:E11">
-    <cfRule type="expression" dxfId="95" priority="25">
-      <formula>LOWER($E11)="critical"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="94" priority="26">
-      <formula>LOWER($E11)="high"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="93" priority="27">
-      <formula>LOWER($E11)="skip"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A12:E12">
-    <cfRule type="expression" dxfId="92" priority="28">
+  <conditionalFormatting sqref="A3:E3">
+    <cfRule type="expression" dxfId="125" priority="1">
+      <formula>LOWER($E3)="critical"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="124" priority="2">
+      <formula>LOWER($E3)="high"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="123" priority="3">
+      <formula>LOWER($E3)="skip"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4:E4">
+    <cfRule type="expression" dxfId="122" priority="4">
+      <formula>LOWER($E4)="critical"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="121" priority="5">
+      <formula>LOWER($E4)="high"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="120" priority="6">
+      <formula>LOWER($E4)="skip"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5:E5">
+    <cfRule type="expression" dxfId="119" priority="7">
+      <formula>LOWER($E5)="critical"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="118" priority="8">
+      <formula>LOWER($E5)="high"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="117" priority="9">
+      <formula>LOWER($E5)="skip"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6:E6">
+    <cfRule type="expression" dxfId="116" priority="10">
+      <formula>LOWER($E6)="critical"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="115" priority="11">
+      <formula>LOWER($E6)="high"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="114" priority="12">
+      <formula>LOWER($E6)="skip"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7:E7">
+    <cfRule type="expression" dxfId="113" priority="13">
+      <formula>LOWER($E7)="critical"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="112" priority="14">
+      <formula>LOWER($E7)="high"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="111" priority="15">
+      <formula>LOWER($E7)="skip"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8:E8">
+    <cfRule type="expression" dxfId="110" priority="16">
+      <formula>LOWER($E8)="critical"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="109" priority="17">
+      <formula>LOWER($E8)="high"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="108" priority="18">
+      <formula>LOWER($E8)="skip"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9:E9">
+    <cfRule type="expression" dxfId="107" priority="19">
+      <formula>LOWER($E9)="critical"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="106" priority="20">
+      <formula>LOWER($E9)="high"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="105" priority="21">
+      <formula>LOWER($E9)="skip"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11:D12">
+    <cfRule type="expression" dxfId="104" priority="46">
+      <formula>LOWER($E10)="critical"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="103" priority="47">
+      <formula>LOWER($E10)="high"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="102" priority="48">
+      <formula>LOWER($E10)="skip"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10:D10 C13">
+    <cfRule type="expression" dxfId="101" priority="52">
       <formula>LOWER($E12)="critical"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="91" priority="29">
+    <cfRule type="expression" dxfId="100" priority="53">
       <formula>LOWER($E12)="high"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="90" priority="30">
+    <cfRule type="expression" dxfId="99" priority="54">
       <formula>LOWER($E12)="skip"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A13:E13">
-    <cfRule type="expression" dxfId="89" priority="31">
-      <formula>LOWER($E13)="critical"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="88" priority="32">
-      <formula>LOWER($E13)="high"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="87" priority="33">
-      <formula>LOWER($E13)="skip"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14:E14">
-    <cfRule type="expression" dxfId="86" priority="34">
-      <formula>LOWER($E14)="critical"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="85" priority="35">
-      <formula>LOWER($E14)="high"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="84" priority="36">
-      <formula>LOWER($E14)="skip"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A15:E15">
-    <cfRule type="expression" dxfId="83" priority="37">
-      <formula>LOWER($E15)="critical"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="82" priority="38">
-      <formula>LOWER($E15)="high"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="81" priority="39">
-      <formula>LOWER($E15)="skip"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A16:E16">
-    <cfRule type="expression" dxfId="80" priority="40">
-      <formula>LOWER($E16)="critical"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="79" priority="41">
-      <formula>LOWER($E16)="high"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="78" priority="42">
-      <formula>LOWER($E16)="skip"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A17:E17">
-    <cfRule type="expression" dxfId="77" priority="43">
+  <conditionalFormatting sqref="B14">
+    <cfRule type="expression" dxfId="2" priority="103">
       <formula>LOWER($E17)="critical"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="44">
+    <cfRule type="expression" dxfId="1" priority="104">
       <formula>LOWER($E17)="high"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="45">
+    <cfRule type="expression" dxfId="0" priority="105">
       <formula>LOWER($E17)="skip"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A18:E18">
-    <cfRule type="expression" dxfId="74" priority="46">
-      <formula>LOWER($E18)="critical"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="73" priority="47">
-      <formula>LOWER($E18)="high"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="72" priority="48">
-      <formula>LOWER($E18)="skip"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A3:E3">
-    <cfRule type="expression" dxfId="71" priority="1">
-      <formula>LOWER($E3)="critical"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="70" priority="2">
-      <formula>LOWER($E3)="high"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="69" priority="3">
-      <formula>LOWER($E3)="skip"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A4:E4">
-    <cfRule type="expression" dxfId="68" priority="4">
-      <formula>LOWER($E4)="critical"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="67" priority="5">
-      <formula>LOWER($E4)="high"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="66" priority="6">
-      <formula>LOWER($E4)="skip"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A5:E5">
-    <cfRule type="expression" dxfId="65" priority="7">
-      <formula>LOWER($E5)="critical"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="64" priority="8">
-      <formula>LOWER($E5)="high"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="63" priority="9">
-      <formula>LOWER($E5)="skip"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A6:E6">
-    <cfRule type="expression" dxfId="62" priority="10">
-      <formula>LOWER($E6)="critical"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="61" priority="11">
-      <formula>LOWER($E6)="high"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="60" priority="12">
-      <formula>LOWER($E6)="skip"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A7:E7">
-    <cfRule type="expression" dxfId="59" priority="13">
-      <formula>LOWER($E7)="critical"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="58" priority="14">
-      <formula>LOWER($E7)="high"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="57" priority="15">
-      <formula>LOWER($E7)="skip"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A8:E8">
-    <cfRule type="expression" dxfId="56" priority="16">
-      <formula>LOWER($E8)="critical"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="55" priority="17">
-      <formula>LOWER($E8)="high"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="54" priority="18">
-      <formula>LOWER($E8)="skip"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9:E9">
-    <cfRule type="expression" dxfId="53" priority="19">
-      <formula>LOWER($E9)="critical"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="52" priority="20">
-      <formula>LOWER($E9)="high"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="51" priority="21">
-      <formula>LOWER($E9)="skip"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="10.6640625" customWidth="1"/>
     <col min="3" max="3" width="50.6640625" customWidth="1"/>
@@ -1697,483 +1811,576 @@
     <col min="5" max="5" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="5">
+        <v>6.9444444444444449E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
-        <f t="shared" ref="A4:A19" si="0">IF(LOWER($E3)="skip",A3,A3+D3)</f>
+        <f t="shared" ref="A4:A15" si="0">IF(LOWER($E3)="skip",A3,A3+D3)</f>
         <v>0.4236111111111111</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="5">
+        <v>1.3888888888888888E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <f t="shared" si="0"/>
-        <v>0.43055555555555552</v>
+        <v>0.4375</v>
       </c>
       <c r="B5" s="1">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="5">
+        <v>1.0416666666666666E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <f t="shared" si="0"/>
-        <v>0.44097222222222221</v>
+        <v>0.44791666666666669</v>
       </c>
       <c r="B6" s="1">
         <v>4</v>
       </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="5">
+        <v>1.3888888888888888E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
-        <v>0.44444444444444442</v>
+        <v>0.46180555555555558</v>
       </c>
       <c r="B7" s="1">
         <v>5</v>
       </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="6">
+        <v>1.3888888888888888E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
-        <v>0.45138888888888884</v>
+        <v>0.47569444444444448</v>
       </c>
       <c r="B8" s="1">
         <v>6</v>
       </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="7">
+        <v>1.3888888888888888E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
-        <v>0.45833333333333326</v>
+        <v>0.48958333333333337</v>
       </c>
       <c r="B9" s="1">
         <v>7</v>
       </c>
-      <c r="C9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="5">
+        <v>6.9444444444444449E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
-        <v>0.46180555555555547</v>
+        <v>0.49652777777777779</v>
       </c>
       <c r="B10" s="1">
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="D10" s="8">
+        <v>2.7777777777777776E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
-        <v>0.46874999999999989</v>
+        <v>0.52430555555555558</v>
       </c>
       <c r="B11" s="1">
         <v>9</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D11" s="5">
+        <v>1.3888888888888888E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
-        <v>0.47916666666666657</v>
+        <v>0.53819444444444442</v>
       </c>
       <c r="B12" s="1">
         <v>10</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D12" s="7">
+        <v>1.3888888888888888E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
-        <v>0.48958333333333326</v>
+        <v>0.55208333333333326</v>
       </c>
       <c r="B13" s="1">
         <v>11</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D13" s="5">
+        <v>6.9444444444444441E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
-        <v>0.51736111111111105</v>
+        <v>0.55902777777777768</v>
       </c>
       <c r="B14" s="1">
         <v>12</v>
       </c>
-      <c r="C14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="7">
+        <v>2.4305555555555556E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
-        <v>0.52430555555555547</v>
+        <v>0.58333333333333326</v>
       </c>
       <c r="B15" s="1">
         <v>13</v>
       </c>
-      <c r="C15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
-        <f t="shared" si="0"/>
-        <v>0.5347222222222221</v>
-      </c>
-      <c r="B16" s="1">
-        <v>14</v>
-      </c>
-      <c r="C16" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
-        <f t="shared" si="0"/>
-        <v>0.54513888888888873</v>
-      </c>
-      <c r="B17" s="1">
-        <v>15</v>
-      </c>
-      <c r="C17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
-        <f t="shared" si="0"/>
-        <v>0.55208333333333315</v>
-      </c>
-      <c r="B18" s="1">
-        <v>16</v>
-      </c>
-      <c r="C18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
-        <f>IF(LOWER($E18)="skip",A18,A18+D18)</f>
-        <v>0.55902777777777757</v>
-      </c>
-      <c r="B19" s="1">
-        <v>17</v>
-      </c>
-      <c r="C19" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
-        <f>IF(LOWER($E19)="skip",A19,A19+D19)</f>
-        <v>0.58333333333333315</v>
-      </c>
-      <c r="C20" t="s">
-        <v>26</v>
+      <c r="C15" s="9" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A10:E10">
-    <cfRule type="expression" dxfId="50" priority="22">
+  <conditionalFormatting sqref="A10 E10">
+    <cfRule type="expression" dxfId="98" priority="82">
       <formula>LOWER($E10)="critical"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="23">
+    <cfRule type="expression" dxfId="97" priority="83">
       <formula>LOWER($E10)="high"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="24">
+    <cfRule type="expression" dxfId="96" priority="84">
       <formula>LOWER($E10)="skip"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A11:E11">
-    <cfRule type="expression" dxfId="47" priority="25">
+  <conditionalFormatting sqref="A11 E11">
+    <cfRule type="expression" dxfId="95" priority="85">
       <formula>LOWER($E11)="critical"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="26">
+    <cfRule type="expression" dxfId="94" priority="86">
       <formula>LOWER($E11)="high"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="27">
+    <cfRule type="expression" dxfId="93" priority="87">
       <formula>LOWER($E11)="skip"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A12:E12">
-    <cfRule type="expression" dxfId="44" priority="28">
+  <conditionalFormatting sqref="A12 E12">
+    <cfRule type="expression" dxfId="92" priority="88">
       <formula>LOWER($E12)="critical"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="29">
+    <cfRule type="expression" dxfId="91" priority="89">
       <formula>LOWER($E12)="high"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="30">
+    <cfRule type="expression" dxfId="90" priority="90">
       <formula>LOWER($E12)="skip"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A13:E13">
-    <cfRule type="expression" dxfId="41" priority="31">
+  <conditionalFormatting sqref="A13 E13">
+    <cfRule type="expression" dxfId="89" priority="91">
       <formula>LOWER($E13)="critical"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="32">
+    <cfRule type="expression" dxfId="88" priority="92">
       <formula>LOWER($E13)="high"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="33">
+    <cfRule type="expression" dxfId="87" priority="93">
       <formula>LOWER($E13)="skip"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A14:E14">
-    <cfRule type="expression" dxfId="38" priority="34">
+  <conditionalFormatting sqref="E14 A14:A15">
+    <cfRule type="expression" dxfId="86" priority="94">
       <formula>LOWER($E14)="critical"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="35">
+    <cfRule type="expression" dxfId="85" priority="95">
       <formula>LOWER($E14)="high"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="36">
+    <cfRule type="expression" dxfId="84" priority="96">
       <formula>LOWER($E14)="skip"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A15:E15">
-    <cfRule type="expression" dxfId="35" priority="37">
+  <conditionalFormatting sqref="E15">
+    <cfRule type="expression" dxfId="83" priority="97">
       <formula>LOWER($E15)="critical"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="38">
+    <cfRule type="expression" dxfId="82" priority="98">
       <formula>LOWER($E15)="high"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="39">
+    <cfRule type="expression" dxfId="81" priority="99">
       <formula>LOWER($E15)="skip"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A16:E16">
-    <cfRule type="expression" dxfId="32" priority="40">
+  <conditionalFormatting sqref="E16">
+    <cfRule type="expression" dxfId="80" priority="100">
       <formula>LOWER($E16)="critical"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="41">
+    <cfRule type="expression" dxfId="79" priority="101">
       <formula>LOWER($E16)="high"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="42">
+    <cfRule type="expression" dxfId="78" priority="102">
       <formula>LOWER($E16)="skip"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A17:E17">
-    <cfRule type="expression" dxfId="29" priority="43">
-      <formula>LOWER($E17)="critical"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="28" priority="44">
-      <formula>LOWER($E17)="high"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="27" priority="45">
-      <formula>LOWER($E17)="skip"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A18:E18">
-    <cfRule type="expression" dxfId="26" priority="46">
-      <formula>LOWER($E18)="critical"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="25" priority="47">
-      <formula>LOWER($E18)="high"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="24" priority="48">
-      <formula>LOWER($E18)="skip"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A19:E19 A20">
-    <cfRule type="expression" dxfId="23" priority="49">
-      <formula>LOWER($E19)="critical"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="22" priority="50">
-      <formula>LOWER($E19)="high"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="21" priority="51">
-      <formula>LOWER($E19)="skip"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A3:E3">
-    <cfRule type="expression" dxfId="20" priority="1">
+  <conditionalFormatting sqref="A3 E3">
+    <cfRule type="expression" dxfId="77" priority="61">
       <formula>LOWER($E3)="critical"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="2">
+    <cfRule type="expression" dxfId="76" priority="62">
       <formula>LOWER($E3)="high"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="3">
+    <cfRule type="expression" dxfId="75" priority="63">
       <formula>LOWER($E3)="skip"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4:E4">
-    <cfRule type="expression" dxfId="17" priority="4">
+  <conditionalFormatting sqref="A4 E4">
+    <cfRule type="expression" dxfId="74" priority="64">
       <formula>LOWER($E4)="critical"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="5">
+    <cfRule type="expression" dxfId="73" priority="65">
       <formula>LOWER($E4)="high"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="6">
+    <cfRule type="expression" dxfId="72" priority="66">
       <formula>LOWER($E4)="skip"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:E5">
-    <cfRule type="expression" dxfId="14" priority="7">
+  <conditionalFormatting sqref="A5 E5">
+    <cfRule type="expression" dxfId="71" priority="67">
       <formula>LOWER($E5)="critical"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="8">
+    <cfRule type="expression" dxfId="70" priority="68">
       <formula>LOWER($E5)="high"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="9">
+    <cfRule type="expression" dxfId="69" priority="69">
       <formula>LOWER($E5)="skip"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A6:E6">
-    <cfRule type="expression" dxfId="11" priority="10">
+  <conditionalFormatting sqref="A6 E6">
+    <cfRule type="expression" dxfId="68" priority="70">
       <formula>LOWER($E6)="critical"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="11">
+    <cfRule type="expression" dxfId="67" priority="71">
       <formula>LOWER($E6)="high"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="12">
+    <cfRule type="expression" dxfId="66" priority="72">
       <formula>LOWER($E6)="skip"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A7:E7">
-    <cfRule type="expression" dxfId="8" priority="13">
+  <conditionalFormatting sqref="A7 E7">
+    <cfRule type="expression" dxfId="65" priority="73">
       <formula>LOWER($E7)="critical"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="14">
+    <cfRule type="expression" dxfId="64" priority="74">
       <formula>LOWER($E7)="high"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="15">
+    <cfRule type="expression" dxfId="63" priority="75">
       <formula>LOWER($E7)="skip"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A8:E8">
-    <cfRule type="expression" dxfId="5" priority="16">
+  <conditionalFormatting sqref="A8 E8">
+    <cfRule type="expression" dxfId="62" priority="76">
       <formula>LOWER($E8)="critical"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="17">
+    <cfRule type="expression" dxfId="61" priority="77">
       <formula>LOWER($E8)="high"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="18">
+    <cfRule type="expression" dxfId="60" priority="78">
       <formula>LOWER($E8)="skip"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A9:E9">
-    <cfRule type="expression" dxfId="2" priority="19">
+  <conditionalFormatting sqref="A9 E9">
+    <cfRule type="expression" dxfId="59" priority="79">
       <formula>LOWER($E9)="critical"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="20">
+    <cfRule type="expression" dxfId="58" priority="80">
       <formula>LOWER($E9)="high"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="21">
+    <cfRule type="expression" dxfId="57" priority="81">
+      <formula>LOWER($E9)="skip"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B10:B15">
+    <cfRule type="expression" dxfId="56" priority="52">
+      <formula>LOWER($E10)="critical"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="55" priority="53">
+      <formula>LOWER($E10)="high"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="54" priority="54">
+      <formula>LOWER($E10)="skip"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3">
+    <cfRule type="expression" dxfId="53" priority="31">
+      <formula>LOWER($E3)="critical"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="52" priority="32">
+      <formula>LOWER($E3)="high"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="51" priority="33">
+      <formula>LOWER($E3)="skip"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4">
+    <cfRule type="expression" dxfId="50" priority="34">
+      <formula>LOWER($E4)="critical"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="49" priority="35">
+      <formula>LOWER($E4)="high"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="48" priority="36">
+      <formula>LOWER($E4)="skip"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5">
+    <cfRule type="expression" dxfId="47" priority="37">
+      <formula>LOWER($E5)="critical"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="46" priority="38">
+      <formula>LOWER($E5)="high"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="45" priority="39">
+      <formula>LOWER($E5)="skip"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6">
+    <cfRule type="expression" dxfId="44" priority="40">
+      <formula>LOWER($E6)="critical"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="43" priority="41">
+      <formula>LOWER($E6)="high"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="42" priority="42">
+      <formula>LOWER($E6)="skip"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7">
+    <cfRule type="expression" dxfId="41" priority="43">
+      <formula>LOWER($E7)="critical"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="40" priority="44">
+      <formula>LOWER($E7)="high"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="39" priority="45">
+      <formula>LOWER($E7)="skip"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8">
+    <cfRule type="expression" dxfId="38" priority="46">
+      <formula>LOWER($E8)="critical"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="37" priority="47">
+      <formula>LOWER($E8)="high"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="36" priority="48">
+      <formula>LOWER($E8)="skip"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9">
+    <cfRule type="expression" dxfId="35" priority="49">
+      <formula>LOWER($E9)="critical"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="34" priority="50">
+      <formula>LOWER($E9)="high"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="33" priority="51">
+      <formula>LOWER($E9)="skip"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11:D12">
+    <cfRule type="expression" dxfId="32" priority="25">
+      <formula>LOWER($E10)="critical"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="31" priority="26">
+      <formula>LOWER($E10)="high"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="30" priority="27">
+      <formula>LOWER($E10)="skip"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10:D10 C13">
+    <cfRule type="expression" dxfId="29" priority="28">
+      <formula>LOWER($E12)="critical"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="29">
+      <formula>LOWER($E12)="high"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="27" priority="30">
+      <formula>LOWER($E12)="skip"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10:D10 D13:D14">
+    <cfRule type="expression" dxfId="26" priority="22">
+      <formula>LOWER($E10)="critical"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="23">
+      <formula>LOWER($E10)="high"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="24">
+      <formula>LOWER($E10)="skip"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:D3">
+    <cfRule type="expression" dxfId="23" priority="1">
+      <formula>LOWER($E3)="critical"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="2">
+      <formula>LOWER($E3)="high"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="3">
+      <formula>LOWER($E3)="skip"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4:D4">
+    <cfRule type="expression" dxfId="20" priority="4">
+      <formula>LOWER($E4)="critical"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="5">
+      <formula>LOWER($E4)="high"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="6">
+      <formula>LOWER($E4)="skip"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5:D5">
+    <cfRule type="expression" dxfId="17" priority="7">
+      <formula>LOWER($E5)="critical"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="8">
+      <formula>LOWER($E5)="high"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="15" priority="9">
+      <formula>LOWER($E5)="skip"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6:D6">
+    <cfRule type="expression" dxfId="14" priority="10">
+      <formula>LOWER($E6)="critical"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="11">
+      <formula>LOWER($E6)="high"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="12">
+      <formula>LOWER($E6)="skip"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7:D7">
+    <cfRule type="expression" dxfId="11" priority="13">
+      <formula>LOWER($E7)="critical"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="14">
+      <formula>LOWER($E7)="high"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="15">
+      <formula>LOWER($E7)="skip"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8:D8">
+    <cfRule type="expression" dxfId="8" priority="16">
+      <formula>LOWER($E8)="critical"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="17">
+      <formula>LOWER($E8)="high"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="18">
+      <formula>LOWER($E8)="skip"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9:D9">
+    <cfRule type="expression" dxfId="5" priority="19">
+      <formula>LOWER($E9)="critical"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="20">
+      <formula>LOWER($E9)="high"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="21">
       <formula>LOWER($E9)="skip"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>